<commit_message>
PO Report Generation has been completed
</commit_message>
<xml_diff>
--- a/VehicleTracker.WebApi/ExcelTemplates/Purchase-Order-Template.xlsx
+++ b/VehicleTracker.WebApi/ExcelTemplates/Purchase-Order-Template.xlsx
@@ -5,21 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MySelf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dynami\Products\VT\VM\VehicleTracker.WebApi\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9C6BE9-A325-46AF-ADAD-7C8902F8F6E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2760150-924A-4863-91DE-DF3913CA2103}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15540" yWindow="450" windowWidth="19620" windowHeight="20790" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BLANK - Purchase Order" sheetId="5" r:id="rId1"/>
+    <sheet name="Purchase-Order" sheetId="5" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'BLANK - Purchase Order'!$B$1:$F$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Purchase-Order'!$B$1:$F$53</definedName>
     <definedName name="Type" localSheetId="0">'[1]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Company Name</t>
   </si>
@@ -99,27 +99,6 @@
   </si>
   <si>
     <t>THANK YOU</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t>Please make check payable to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Your Company Name.</t>
-    </r>
   </si>
   <si>
     <t>PURCHASE ORDER NO.</t>
@@ -191,19 +170,16 @@
     <t>AUTHORIZED SIGNATURE</t>
   </si>
   <si>
-    <t>For questions concerning this invoice, please contact</t>
-  </si>
-  <si>
     <t>Name, (321) 456-7890, Email Address</t>
-  </si>
-  <si>
-    <t>www.yourwebaddress.com</t>
   </si>
   <si>
     <t>YOUR LOGO</t>
   </si>
   <si>
     <t>PURCHASE ORDER</t>
+  </si>
+  <si>
+    <t>For questions concerning this purchasing order, please contact our purchasing department</t>
   </si>
 </sst>
 </file>
@@ -217,7 +193,7 @@
     <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -267,12 +243,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
@@ -314,13 +284,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
       <sz val="8"/>
       <color theme="4" tint="-0.499984740745262"/>
       <name val="Century Gothic"/>
@@ -408,6 +371,12 @@
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -423,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -503,6 +472,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -512,7 +499,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -522,135 +509,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="21" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -966,588 +975,559 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G929"/>
+  <dimension ref="A1:G935"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="41.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="5" customWidth="1"/>
     <col min="5" max="6" width="17.7109375" style="5" customWidth="1"/>
-    <col min="7" max="8" width="3" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="3" style="5" customWidth="1"/>
     <col min="9" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="88.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="46" t="s">
-        <v>36</v>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="88.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="40" t="s">
+        <v>33</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="53" t="s">
-        <v>37</v>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="51" t="s">
+        <v>34</v>
       </c>
-      <c r="F1" s="53"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="51"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="7"/>
-      <c r="F2" s="27" t="s">
+      <c r="E2" s="63" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="63"/>
+    </row>
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="56"/>
       <c r="D3" s="7"/>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="46"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="7"/>
-      <c r="F4" s="27" t="s">
-        <v>22</v>
+      <c r="E4" s="63" t="s">
+        <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="63"/>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="7"/>
-      <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="7"/>
-      <c r="F6" s="27" t="s">
+      <c r="E6" s="64" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="64"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="7"/>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="48"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="14"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="E9" s="15" t="s">
+      <c r="C9" s="12"/>
+      <c r="E9" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="E10" s="17" t="s">
+      <c r="C10" s="57"/>
+      <c r="E10" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+    </row>
+    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="E11" s="7" t="s">
+      <c r="C11" s="58"/>
+      <c r="E11" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="E12" s="7" t="s">
+      <c r="C12" s="58"/>
+      <c r="E12" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="28"/>
-    </row>
-    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="E13" s="7" t="s">
+      <c r="C13" s="58"/>
+      <c r="E13" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="E14" s="7" t="s">
+      <c r="C14" s="58"/>
+      <c r="E14" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-    </row>
-    <row r="16" spans="1:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="58"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+    </row>
+    <row r="18" spans="1:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="D19" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="37" t="s">
+      <c r="F19" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="37" t="s">
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" spans="1:7" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" spans="1:7" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="19"/>
+    </row>
+    <row r="33" spans="1:7" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="19"/>
+    </row>
+    <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="19"/>
+    </row>
+    <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="19"/>
+    </row>
+    <row r="36" spans="1:7" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="19"/>
+    </row>
+    <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="E38" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="25">
+        <f>SUM(F23:F37)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="20"/>
+    </row>
+    <row r="39" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="25">
+        <v>0</v>
+      </c>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="E40" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="25">
+        <f>F38-F39</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="20"/>
+    </row>
+    <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="E41" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="28">
+        <v>0</v>
+      </c>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="E42" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="25">
+        <f>F40*F41</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="E43" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="26">
+        <v>0</v>
+      </c>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="30"/>
+      <c r="E44" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="26">
+        <v>0</v>
+      </c>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="45" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="53"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="27">
+        <f>SUM(F40,F42,F43,F44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
-    </row>
-    <row r="19" spans="1:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="27" t="s">
-        <v>12</v>
+      <c r="C48" s="41"/>
+      <c r="E48" s="14" t="s">
+        <v>1</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>13</v>
+      <c r="F48" s="42"/>
+    </row>
+    <row r="49" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="23"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="15"/>
+    </row>
+    <row r="50" spans="1:7" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+    </row>
+    <row r="51" spans="1:7" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="B51" s="54" t="s">
+        <v>35</v>
       </c>
-      <c r="D20" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24">
-        <f t="shared" ref="F21:F24" si="0">D21*E21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9">
-        <f t="shared" ref="F25:F31" si="1">D25*E25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="E32" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="31">
-        <f>SUM(F21:F31)</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="25"/>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="31">
-        <v>0</v>
-      </c>
-      <c r="G33" s="26"/>
-    </row>
-    <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="E34" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="31">
-        <f>F32-F33</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="25"/>
-    </row>
-    <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="E35" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="34">
-        <v>0</v>
-      </c>
-      <c r="G35" s="25"/>
-    </row>
-    <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="E36" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="31">
-        <f>F34*F35</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="25"/>
-    </row>
-    <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="E37" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="32">
-        <v>0</v>
-      </c>
-      <c r="G37" s="25"/>
-    </row>
-    <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="36"/>
-      <c r="E38" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="32">
-        <v>0</v>
-      </c>
-      <c r="G38" s="25"/>
-    </row>
-    <row r="39" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="33">
-        <f>SUM(F34,F36,F37,F38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="15" t="s">
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+    </row>
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="B52" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="47"/>
-      <c r="E42" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F42" s="48"/>
-    </row>
-    <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="28"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-    </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="B45" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-    </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="B46" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-    </row>
-    <row r="47" spans="1:7" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-    </row>
-    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+    </row>
+    <row r="53" spans="1:7" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
     </row>
     <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
@@ -9420,6 +9400,8 @@
       <c r="B928" s="1"/>
       <c r="C928" s="3"/>
       <c r="D928" s="1"/>
+      <c r="E928" s="1"/>
+      <c r="F928" s="1"/>
       <c r="G928" s="1"/>
     </row>
     <row r="929" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -9427,21 +9409,98 @@
       <c r="B929" s="1"/>
       <c r="C929" s="3"/>
       <c r="D929" s="1"/>
+      <c r="E929" s="1"/>
+      <c r="F929" s="1"/>
       <c r="G929" s="1"/>
     </row>
+    <row r="930" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A930" s="1"/>
+      <c r="B930" s="1"/>
+      <c r="C930" s="3"/>
+      <c r="D930" s="1"/>
+      <c r="E930" s="1"/>
+      <c r="F930" s="1"/>
+      <c r="G930" s="1"/>
+    </row>
+    <row r="931" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A931" s="1"/>
+      <c r="B931" s="1"/>
+      <c r="C931" s="3"/>
+      <c r="D931" s="1"/>
+      <c r="E931" s="1"/>
+      <c r="F931" s="1"/>
+      <c r="G931" s="1"/>
+    </row>
+    <row r="932" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A932" s="1"/>
+      <c r="B932" s="1"/>
+      <c r="C932" s="3"/>
+      <c r="D932" s="1"/>
+      <c r="E932" s="1"/>
+      <c r="F932" s="1"/>
+      <c r="G932" s="1"/>
+    </row>
+    <row r="933" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A933" s="1"/>
+      <c r="B933" s="1"/>
+      <c r="C933" s="3"/>
+      <c r="D933" s="1"/>
+      <c r="E933" s="1"/>
+      <c r="F933" s="1"/>
+      <c r="G933" s="1"/>
+    </row>
+    <row r="934" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A934" s="1"/>
+      <c r="B934" s="1"/>
+      <c r="C934" s="3"/>
+      <c r="D934" s="1"/>
+      <c r="G934" s="1"/>
+    </row>
+    <row r="935" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A935" s="1"/>
+      <c r="B935" s="1"/>
+      <c r="C935" s="3"/>
+      <c r="D935" s="1"/>
+      <c r="G935" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
+  <mergeCells count="32">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B33:C37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B39:C43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup scale="89" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="79" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>